<commit_message>
Model #1 sequence change
</commit_message>
<xml_diff>
--- a/model1_data.xlsx
+++ b/model1_data.xlsx
@@ -34,23 +34,23 @@
     <t>B</t>
   </si>
   <si>
-    <t>C</t>
+    <t>F</t>
   </si>
   <si>
-    <t>D</t>
+    <t>C</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>F</t>
+    <t>D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -60,7 +60,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -76,14 +75,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -340,7 +336,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>2.0</v>
       </c>
       <c r="C3" s="1">
@@ -357,7 +353,7 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>3.0</v>
       </c>
       <c r="C4" s="1">
@@ -374,7 +370,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>4.0</v>
       </c>
       <c r="C5" s="1">
@@ -391,7 +387,7 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>5.0</v>
       </c>
       <c r="C6" s="1">
@@ -408,7 +404,7 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>6.0</v>
       </c>
       <c r="C7" s="1">
@@ -644,9 +640,9 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
         <v>2.0</v>
       </c>
       <c r="C21" s="1">
@@ -661,9 +657,9 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1">
         <v>3.0</v>
       </c>
       <c r="C22" s="1">
@@ -678,9 +674,9 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="2">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
         <v>4.0</v>
       </c>
       <c r="C23" s="1">
@@ -695,9 +691,9 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1">
         <v>5.0</v>
       </c>
       <c r="C24" s="1">
@@ -712,9 +708,9 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="2">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1">
         <v>6.0</v>
       </c>
       <c r="C25" s="1">
@@ -731,7 +727,7 @@
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>1.0</v>
       </c>
       <c r="C26" s="1">
@@ -746,9 +742,9 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="2">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1">
         <v>2.0</v>
       </c>
       <c r="C27" s="1">
@@ -763,9 +759,9 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="2">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
         <v>3.0</v>
       </c>
       <c r="C28" s="1">
@@ -780,9 +776,9 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="2">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1">
         <v>4.0</v>
       </c>
       <c r="C29" s="1">
@@ -797,9 +793,9 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1">
@@ -814,9 +810,9 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="2">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1">
         <v>6.0</v>
       </c>
       <c r="C31" s="1">
@@ -833,7 +829,7 @@
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>1.0</v>
       </c>
       <c r="C32" s="1">
@@ -848,9 +844,9 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="2">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
         <v>2.0</v>
       </c>
       <c r="C33" s="1">
@@ -865,9 +861,9 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="2">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
         <v>3.0</v>
       </c>
       <c r="C34" s="1">
@@ -882,9 +878,9 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="2">
+        <v>10</v>
+      </c>
+      <c r="B35" s="1">
         <v>4.0</v>
       </c>
       <c r="C35" s="1">
@@ -899,9 +895,9 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="2">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1">
         <v>5.0</v>
       </c>
       <c r="C36" s="1">
@@ -916,9 +912,9 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="2">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
         <v>6.0</v>
       </c>
       <c r="C37" s="1">
@@ -933,7 +929,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1">
         <v>1.0</v>
@@ -950,7 +946,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B39" s="1">
         <v>2.0</v>
@@ -984,7 +980,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1">
         <v>4.0</v>
@@ -1001,7 +997,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1">
         <v>5.0</v>
@@ -1018,7 +1014,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" s="1">
         <v>6.0</v>
@@ -1035,7 +1031,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B44" s="1">
         <v>1.0</v>
@@ -1052,7 +1048,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B45" s="1">
         <v>2.0</v>
@@ -1086,7 +1082,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" s="1">
         <v>4.0</v>
@@ -1103,7 +1099,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B48" s="1">
         <v>5.0</v>
@@ -1120,7 +1116,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49" s="1">
         <v>6.0</v>
@@ -1137,7 +1133,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B50" s="1">
         <v>1.0</v>
@@ -1154,7 +1150,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B51" s="1">
         <v>2.0</v>
@@ -1188,7 +1184,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B53" s="1">
         <v>4.0</v>
@@ -1205,7 +1201,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B54" s="1">
         <v>5.0</v>
@@ -1222,7 +1218,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B55" s="1">
         <v>6.0</v>
@@ -1239,7 +1235,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1">
         <v>1.0</v>
@@ -1256,7 +1252,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B57" s="1">
         <v>2.0</v>
@@ -1273,7 +1269,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" s="1">
         <v>3.0</v>
@@ -1290,7 +1286,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B59" s="1">
         <v>4.0</v>
@@ -1307,7 +1303,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B60" s="1">
         <v>5.0</v>
@@ -1324,7 +1320,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61" s="1">
         <v>6.0</v>
@@ -1341,7 +1337,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B62" s="1">
         <v>1.0</v>
@@ -1358,7 +1354,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B63" s="1">
         <v>2.0</v>
@@ -1375,7 +1371,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64" s="1">
         <v>3.0</v>
@@ -1392,7 +1388,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B65" s="1">
         <v>4.0</v>
@@ -1409,7 +1405,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1">
         <v>5.0</v>
@@ -1426,7 +1422,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B67" s="1">
         <v>6.0</v>
@@ -1443,7 +1439,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B68" s="1">
         <v>1.0</v>
@@ -1460,7 +1456,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B69" s="1">
         <v>2.0</v>
@@ -1477,7 +1473,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70" s="1">
         <v>3.0</v>
@@ -1494,7 +1490,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B71" s="1">
         <v>4.0</v>
@@ -1511,7 +1507,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B72" s="1">
         <v>5.0</v>
@@ -1528,7 +1524,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73" s="1">
         <v>6.0</v>
@@ -1562,7 +1558,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B75" s="1">
         <v>2.0</v>
@@ -1579,7 +1575,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B76" s="1">
         <v>3.0</v>
@@ -1596,7 +1592,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B77" s="1">
         <v>4.0</v>
@@ -1613,7 +1609,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B78" s="1">
         <v>5.0</v>
@@ -1630,7 +1626,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1">
         <v>6.0</v>
@@ -1664,7 +1660,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B81" s="1">
         <v>2.0</v>
@@ -1681,7 +1677,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B82" s="1">
         <v>3.0</v>
@@ -1698,7 +1694,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B83" s="1">
         <v>4.0</v>
@@ -1715,7 +1711,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B84" s="1">
         <v>5.0</v>
@@ -1732,7 +1728,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B85" s="1">
         <v>6.0</v>
@@ -1766,7 +1762,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B87" s="1">
         <v>2.0</v>
@@ -1783,7 +1779,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B88" s="1">
         <v>3.0</v>
@@ -1800,7 +1796,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B89" s="1">
         <v>4.0</v>
@@ -1817,7 +1813,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B90" s="1">
         <v>5.0</v>
@@ -1834,7 +1830,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B91" s="1">
         <v>6.0</v>
@@ -1851,7 +1847,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B92" s="1">
         <v>1.0</v>
@@ -1868,7 +1864,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B93" s="1">
         <v>2.0</v>
@@ -1885,7 +1881,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B94" s="1">
         <v>3.0</v>
@@ -1902,7 +1898,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B95" s="1">
         <v>4.0</v>
@@ -1919,7 +1915,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B96" s="1">
         <v>5.0</v>
@@ -1936,7 +1932,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B97" s="1">
         <v>6.0</v>
@@ -1953,7 +1949,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B98" s="1">
         <v>1.0</v>
@@ -1970,7 +1966,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B99" s="1">
         <v>2.0</v>
@@ -1987,7 +1983,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B100" s="1">
         <v>3.0</v>
@@ -2004,7 +2000,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B101" s="1">
         <v>4.0</v>
@@ -2021,7 +2017,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B102" s="1">
         <v>5.0</v>
@@ -2038,7 +2034,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B103" s="1">
         <v>6.0</v>
@@ -2055,7 +2051,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B104" s="1">
         <v>1.0</v>
@@ -2072,7 +2068,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B105" s="1">
         <v>2.0</v>
@@ -2089,7 +2085,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B106" s="1">
         <v>3.0</v>
@@ -2106,7 +2102,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B107" s="1">
         <v>4.0</v>
@@ -2123,7 +2119,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B108" s="1">
         <v>5.0</v>
@@ -2140,7 +2136,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B109" s="1">
         <v>6.0</v>

</xml_diff>